<commit_message>
Figure updates and such
</commit_message>
<xml_diff>
--- a/Pictures/Number of robots.xlsx
+++ b/Pictures/Number of robots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\UT AUSTIN\Sha Lab\Research\Placement\Placement\Pictures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BF15EA7-6CAC-4CBB-B383-0A62DA3E2941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D191867-5752-4D01-B232-650C6C40B8B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6330" yWindow="3960" windowWidth="28800" windowHeight="15435" xr2:uid="{A020482A-4D80-4C90-BAF1-E63680C2BEE2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A020482A-4D80-4C90-BAF1-E63680C2BEE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -90,7 +90,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -223,6 +223,56 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.21687691921666089"/>
+                  <c:y val="2.3094654191689558E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$9</c:f>
@@ -1491,7 +1541,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>